<commit_message>
[0.0.2] Improved search and information counting
</commit_message>
<xml_diff>
--- a/plans/dados.xlsx
+++ b/plans/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dawtonico\apps\projects\sync_excel\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A328818-5398-4561-9115-99636C981F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8B92E9-1DD0-4295-AF0F-0C65EF24F347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7FD06F14-B117-4412-8760-5CAC0AB67154}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>start_date</t>
   </si>
@@ -56,30 +56,6 @@
     <t>end_hour</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
-    <t>CONSULTA: PSICOLOGIA - SALA: 01</t>
-  </si>
-  <si>
-    <t>CONSULTA: DERMATOLOGIA - SALA: 03</t>
-  </si>
-  <si>
-    <t>EXAME: LABORATORIO - LAB: 01</t>
-  </si>
-  <si>
-    <t>0004</t>
-  </si>
-  <si>
-    <t>CONSULTA: PSICOLOGIA - SALA: 02</t>
-  </si>
-  <si>
     <t>05/10/2023</t>
   </si>
   <si>
@@ -95,41 +71,47 @@
     <t>responsible</t>
   </si>
   <si>
-    <t>Dr. Yasmin Pereira</t>
-  </si>
-  <si>
-    <t>Dr. Angela Jaqueline</t>
-  </si>
-  <si>
-    <t>Dr. Pedro Miguel</t>
-  </si>
-  <si>
-    <t>0005</t>
-  </si>
-  <si>
-    <t>0006</t>
-  </si>
-  <si>
-    <t>0007</t>
-  </si>
-  <si>
-    <t>13:30:00</t>
-  </si>
-  <si>
-    <t>0008</t>
-  </si>
-  <si>
-    <t>0009</t>
-  </si>
-  <si>
-    <t>EXAME: LABORATORIO - LAB: 02</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>00001-00-0000</t>
+  </si>
+  <si>
+    <t>00002-00-0000</t>
+  </si>
+  <si>
+    <t>00003-00-0000</t>
+  </si>
+  <si>
+    <t>00004-00-0000</t>
+  </si>
+  <si>
+    <t>06/10/2023</t>
+  </si>
+  <si>
+    <t>01/10/2023</t>
+  </si>
+  <si>
+    <t>RECICLAGEM: PRODUTO - TREINAMENTO - SITE</t>
+  </si>
+  <si>
+    <t>MIGRAÇÃO: PRODUTO - TREINAMENTO - SITE</t>
+  </si>
+  <si>
+    <t>ETAPA TÉCNICA: PRODUTO - TREINAMENTO - SITE</t>
+  </si>
+  <si>
+    <t>ETAPA TÉCNICA: PRODUTO - TREINAMENTO - SITE - J.A</t>
+  </si>
+  <si>
+    <t>INSTRUTOR(A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +123,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -500,249 +488,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9ED322-2002-4D95-825A-BE52EC7CB55A}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="40.7109375" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.7109375" style="4"/>
+    <col min="2" max="2" width="52.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1"/>
+    <col min="4" max="7" width="13.7109375" style="4"/>
+    <col min="8" max="8" width="22.28515625" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="13.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C2" s="1" t="str">
+        <f>IFERROR(LEFT(B2,FIND(":",B2)-1),"")</f>
+        <v>RECICLAGEM</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C66" si="0">IFERROR(LEFT(B3,FIND(":",B3)-1),"")</f>
+        <v>MIGRAÇÃO</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ETAPA TÉCNICA</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ETAPA TÉCNICA</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>